<commit_message>
create test for ConnectionRecord Properties data types and value
</commit_message>
<xml_diff>
--- a/tests/db_files/db.xlsx
+++ b/tests/db_files/db.xlsx
@@ -291,7 +291,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="118">
   <si>
     <t>Description</t>
   </si>
@@ -730,9 +730,6 @@
     <t>COM2</t>
   </si>
   <si>
-    <t>baud_rate=119200</t>
-  </si>
-  <si>
     <t>USB::0x1234::125::A22-5::INSTR</t>
   </si>
   <si>
@@ -743,9 +740,6 @@
   </si>
   <si>
     <t>ASRL1::INSTR</t>
-  </si>
-  <si>
-    <t>alias=DUT</t>
   </si>
   <si>
     <t>GPIB::3</t>
@@ -820,6 +814,9 @@
   </si>
   <si>
     <t>baud_rate=9600; write_termination=\n; read_termination=\r\n</t>
+  </si>
+  <si>
+    <t>a=1; b=1.1; c=true; d=True; e=false; f=False; g=None; h=; i=\n; j=\r; k=\r\n; l=some text; m=D:\Data\</t>
   </si>
 </sst>
 </file>
@@ -1347,7 +1344,7 @@
         <v>15</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1416,7 +1413,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>58</v>
@@ -1790,7 +1787,7 @@
         <v>40129</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>18</v>
@@ -1836,10 +1833,10 @@
         <v>7</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D19" s="23">
         <v>37871232</v>
@@ -1848,10 +1845,10 @@
         <v>5</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1868,7 +1865,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,7 +1875,7 @@
     <col min="3" max="3" width="13.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="86.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="62.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="89.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9.140625" style="16"/>
     <col min="9" max="9" width="43.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="16"/>
@@ -1912,7 +1909,7 @@
         <v>81</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>87</v>
@@ -1930,7 +1927,7 @@
         <v>82</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>87</v>
@@ -1938,9 +1935,7 @@
       <c r="E3" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="18" t="s">
-        <v>95</v>
-      </c>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
@@ -1956,7 +1951,7 @@
         <v>87</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F4" s="18"/>
     </row>
@@ -1968,13 +1963,13 @@
         <v>84</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>86</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F5" s="18"/>
     </row>
@@ -1986,13 +1981,13 @@
         <v>89</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>87</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F6" s="18"/>
     </row>
@@ -2010,7 +2005,7 @@
         <v>86</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F7" s="18"/>
     </row>
@@ -2022,17 +2017,15 @@
         <v>90</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>87</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>100</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
@@ -2042,13 +2035,13 @@
         <v>92</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>86</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F9" s="18"/>
     </row>
@@ -2066,10 +2059,10 @@
         <v>86</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
@@ -2077,10 +2070,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C11" s="23">
         <v>37871232</v>
@@ -2089,7 +2082,10 @@
         <v>86</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
unify the docstrings and the documentation to make sense together
</commit_message>
<xml_diff>
--- a/tests/db_files/db.xlsx
+++ b/tests/db_files/db.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="0" windowWidth="18255" windowHeight="11955" activeTab="1"/>
+    <workbookView xWindow="15120" yWindow="0" windowWidth="18255" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="Equipment" sheetId="1" r:id="rId1"/>
@@ -787,6 +787,15 @@
     <t>8753ES</t>
   </si>
   <si>
+    <t>DVM</t>
+  </si>
+  <si>
+    <t>baud_rate=9600; write_termination=\n; read_termination=\r\n</t>
+  </si>
+  <si>
+    <t>a=1; b=1.1; c=true; d=True; e=false; f=False; g=None; h=; i=\n; j=\r; k=\r\n; l=some text; m=D:\Data\</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -796,7 +805,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Calibration Period</t>
+      <t xml:space="preserve">Calibration Cycle </t>
     </r>
     <r>
       <rPr>
@@ -806,17 +815,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> [years]</t>
+      <t>[years]</t>
     </r>
-  </si>
-  <si>
-    <t>DVM</t>
-  </si>
-  <si>
-    <t>baud_rate=9600; write_termination=\n; read_termination=\r\n</t>
-  </si>
-  <si>
-    <t>a=1; b=1.1; c=true; d=True; e=false; f=False; g=None; h=; i=\n; j=\r; k=\r\n; l=some text; m=D:\Data\</t>
   </si>
 </sst>
 </file>
@@ -1292,9 +1292,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1344,7 +1344,7 @@
         <v>15</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1787,7 +1787,7 @@
         <v>40129</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>18</v>
@@ -1864,9 +1864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2062,7 +2060,7 @@
         <v>98</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
@@ -2085,7 +2083,7 @@
         <v>109</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use double quotes for read_termination and write_termination in database
</commit_message>
<xml_diff>
--- a/tests/db_files/db.xlsx
+++ b/tests/db_files/db.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.borbely\code\git\msl-equipment\tests\db_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\git\msl-equipment\tests\db_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="0" windowWidth="18255" windowHeight="11955"/>
+    <workbookView xWindow="15120" yWindow="0" windowWidth="18255" windowHeight="11955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Equipment" sheetId="1" r:id="rId1"/>
     <sheet name="Connections" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -790,12 +790,6 @@
     <t>DVM</t>
   </si>
   <si>
-    <t>baud_rate=9600; write_termination=\n; read_termination=\r\n</t>
-  </si>
-  <si>
-    <t>a=1; b=1.1; c=true; d=True; e=false; f=False; g=None; h=; i=\n; j=\r; k=\r\n; l=some text; m=D:\Data\</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -817,6 +811,12 @@
       </rPr>
       <t>[years]</t>
     </r>
+  </si>
+  <si>
+    <t>a=1; b=1.1; c=true; d=True; e=false; f=False; g=None; h=; i="\n"; j="\r"; k="\r\n"; l=some text; m=D:\Data\</t>
+  </si>
+  <si>
+    <t>baud_rate=9600; write_termination="\n"; read_termination="\r\n"</t>
   </si>
 </sst>
 </file>
@@ -1292,27 +1292,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="35.59765625" customWidth="1"/>
+    <col min="3" max="3" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.59765625" customWidth="1"/>
+    <col min="6" max="6" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.3984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="171.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1344,10 +1344,10 @@
         <v>15</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1433,7 +1433,7 @@
       </c>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1515,7 +1515,7 @@
       </c>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -1543,7 +1543,7 @@
       </c>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1625,7 +1625,7 @@
       </c>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -1679,7 +1679,7 @@
       </c>
       <c r="J13" s="11"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
@@ -1739,7 +1739,7 @@
       </c>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
@@ -1828,7 +1828,7 @@
       </c>
       <c r="J18" s="14"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
@@ -1864,22 +1864,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="86.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="89.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="16"/>
-    <col min="9" max="9" width="43.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="25.1328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.3984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.86328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.3984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="86.86328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="89.86328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.1328125" style="16"/>
+    <col min="9" max="9" width="43.3984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1328125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>79</v>
       </c>
@@ -1899,7 +1901,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="18" t="s">
         <v>4</v>
       </c>
@@ -1917,7 +1919,7 @@
       </c>
       <c r="F2" s="18"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="18" t="s">
         <v>83</v>
       </c>
@@ -1935,7 +1937,7 @@
       </c>
       <c r="F3" s="18"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>4</v>
       </c>
@@ -1953,7 +1955,7 @@
       </c>
       <c r="F4" s="18"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="18" t="s">
         <v>85</v>
       </c>
@@ -1971,7 +1973,7 @@
       </c>
       <c r="F5" s="18"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="18" t="s">
         <v>88</v>
       </c>
@@ -1989,7 +1991,7 @@
       </c>
       <c r="F6" s="18"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="21" t="s">
         <v>4</v>
       </c>
@@ -2007,7 +2009,7 @@
       </c>
       <c r="F7" s="18"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="18" t="s">
         <v>17</v>
       </c>
@@ -2025,7 +2027,7 @@
       </c>
       <c r="F8" s="18"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="18" t="s">
         <v>91</v>
       </c>
@@ -2043,7 +2045,7 @@
       </c>
       <c r="F9" s="18"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="19" t="s">
         <v>4</v>
       </c>
@@ -2060,13 +2062,13 @@
         <v>98</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="23" t="s">
         <v>107</v>
       </c>

</xml_diff>

<commit_message>
surround CR and LF characters in double quotes
</commit_message>
<xml_diff>
--- a/tests/db_files/db.xlsx
+++ b/tests/db_files/db.xlsx
@@ -790,12 +790,6 @@
     <t>DVM</t>
   </si>
   <si>
-    <t>baud_rate=9600; write_termination=\n; read_termination=\r\n</t>
-  </si>
-  <si>
-    <t>a=1; b=1.1; c=true; d=True; e=false; f=False; g=None; h=; i=\n; j=\r; k=\r\n; l=some text; m=D:\Data\</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -817,6 +811,12 @@
       </rPr>
       <t>[years]</t>
     </r>
+  </si>
+  <si>
+    <t>baud_rate=9600; write_termination="\n"; read_termination="\r\n"</t>
+  </si>
+  <si>
+    <t>a=1; b=1.1; c=true; d=True; e=false; f=False; g=None; h=; i="\n"; j="\r"; k="\r\n"; l=some text; m=D:\Data\</t>
   </si>
 </sst>
 </file>
@@ -1344,7 +1344,7 @@
         <v>15</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1864,7 +1864,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1873,7 +1875,7 @@
     <col min="3" max="3" width="13.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="86.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="89.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="95.140625" style="16" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9.140625" style="16"/>
     <col min="9" max="9" width="43.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="16"/>
@@ -2060,7 +2062,7 @@
         <v>98</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
@@ -2083,7 +2085,7 @@
         <v>109</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
many changes in this commit
- create utils.py module
- move LR, CR to constants.py
- rename 'type' to 'socket_type' for ConnectionSocket class
- create "user_defined" option for an EquipmentRecord
</commit_message>
<xml_diff>
--- a/tests/db_files/db.xlsx
+++ b/tests/db_files/db.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="0" windowWidth="18255" windowHeight="11955" activeTab="1"/>
+    <workbookView xWindow="15120" yWindow="0" windowWidth="18255" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="Equipment" sheetId="1" r:id="rId1"/>
@@ -813,10 +813,10 @@
     </r>
   </si>
   <si>
-    <t>a=1; b=1.1; c=true; d=True; e=false; f=False; g=None; h=; i="\n"; j="\r"; k="\r\n"; l=some text; m=D:\Data\</t>
-  </si>
-  <si>
     <t>baud_rate=9600; write_termination="\n"; read_termination="\r\n"</t>
+  </si>
+  <si>
+    <t>a=1; b=1.1; c=true; d=True; e=false; f=False; g=None; h=; i_termination=\n; j_termination='\r'; k_termination="\r\n"; l=some text; m=D:\Data\</t>
   </si>
 </sst>
 </file>
@@ -1292,7 +1292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -1864,18 +1864,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.1328125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.3984375" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.86328125" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.3984375" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="86.86328125" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="89.86328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.59765625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="74.796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="113.796875" style="16" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9.1328125" style="16"/>
     <col min="9" max="9" width="43.3984375" style="16" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.1328125" style="16"/>
@@ -2062,7 +2060,7 @@
         <v>98</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
@@ -2085,7 +2083,7 @@
         <v>109</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create Connection.parse_address() and remove some interface aliases
</commit_message>
<xml_diff>
--- a/tests/db_files/db.xlsx
+++ b/tests/db_files/db.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\git\msl-equipment\tests\db_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.borbely\code\git\msl-equipment\tests\db_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16C2982-74D8-4BDE-8852-324D51AA0F21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="0" windowWidth="18255" windowHeight="11955"/>
+    <workbookView xWindow="2475" yWindow="735" windowWidth="25395" windowHeight="14370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipment" sheetId="1" r:id="rId1"/>
@@ -25,13 +26,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Humidity</author>
     <author>Joseph Borbely</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -67,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -93,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -129,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="1" shapeId="0">
+    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -155,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="1" shapeId="0">
+    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -191,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="1" shapeId="0">
+    <comment ref="F1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -271,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="1" shapeId="0">
+    <comment ref="E5" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -736,9 +737,6 @@
     <t>TCPIP::192.168.1.50::INSTR</t>
   </si>
   <si>
-    <t>ENET+GPIB::192.168.1.100+7</t>
-  </si>
-  <si>
     <t>ASRL1::INSTR</t>
   </si>
   <si>
@@ -818,11 +816,14 @@
   <si>
     <t>a=1; b=1.1; c=true; d=True; e=false; f=False; g=None; h=; i_termination=\n; j_termination='\r'; k_termination="\r\n"; l=some text; m=D:\Data\</t>
   </si>
+  <si>
+    <t>Prologix::192.168.1.100::7</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1409]d\ mmmm\ yyyy;@"/>
   </numFmts>
@@ -1289,30 +1290,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="35.59765625" customWidth="1"/>
-    <col min="3" max="3" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.59765625" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.73046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.3984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.1328125" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="171.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1344,10 +1345,10 @@
         <v>15</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1377,7 +1378,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1405,7 +1406,7 @@
       </c>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1413,7 +1414,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>58</v>
@@ -1433,7 +1434,7 @@
       </c>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1459,7 +1460,7 @@
       </c>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1487,7 +1488,7 @@
       </c>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1515,7 +1516,7 @@
       </c>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -1543,7 +1544,7 @@
       </c>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1569,7 +1570,7 @@
       </c>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1597,7 +1598,7 @@
       </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1625,7 +1626,7 @@
       </c>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -1653,7 +1654,7 @@
       </c>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -1679,7 +1680,7 @@
       </c>
       <c r="J13" s="11"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1711,7 +1712,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
@@ -1739,7 +1740,7 @@
       </c>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
@@ -1767,7 +1768,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -1787,7 +1788,7 @@
         <v>40129</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>18</v>
@@ -1802,7 +1803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
@@ -1828,15 +1829,15 @@
       </c>
       <c r="J18" s="14"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="19" t="s">
         <v>107</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>108</v>
       </c>
       <c r="D19" s="23">
         <v>37871232</v>
@@ -1845,14 +1846,14 @@
         <v>5</v>
       </c>
       <c r="H19" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="I19" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="I19" s="19" t="s">
-        <v>111</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J17">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J17">
     <sortCondition ref="H2:H17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1861,25 +1862,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.59765625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="74.796875" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="113.796875" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.1328125" style="16"/>
-    <col min="9" max="9" width="43.3984375" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1328125" style="16"/>
+    <col min="2" max="2" width="17.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="74.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="113.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="16"/>
+    <col min="9" max="9" width="43.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>79</v>
       </c>
@@ -1899,7 +1902,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>4</v>
       </c>
@@ -1907,7 +1910,7 @@
         <v>81</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>87</v>
@@ -1917,7 +1920,7 @@
       </c>
       <c r="F2" s="18"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>83</v>
       </c>
@@ -1925,7 +1928,7 @@
         <v>82</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>87</v>
@@ -1935,7 +1938,7 @@
       </c>
       <c r="F3" s="18"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>4</v>
       </c>
@@ -1953,7 +1956,7 @@
       </c>
       <c r="F4" s="18"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>85</v>
       </c>
@@ -1961,17 +1964,17 @@
         <v>84</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>86</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F5" s="18"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>88</v>
       </c>
@@ -1979,7 +1982,7 @@
         <v>89</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>87</v>
@@ -1989,7 +1992,7 @@
       </c>
       <c r="F6" s="18"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>4</v>
       </c>
@@ -2003,11 +2006,11 @@
         <v>86</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="F7" s="18"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>17</v>
       </c>
@@ -2015,17 +2018,17 @@
         <v>90</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>87</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F8" s="18"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>91</v>
       </c>
@@ -2033,17 +2036,17 @@
         <v>92</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>86</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F9" s="18"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>4</v>
       </c>
@@ -2057,21 +2060,21 @@
         <v>86</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>107</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>108</v>
       </c>
       <c r="C11" s="23">
         <v>37871232</v>
@@ -2080,10 +2083,10 @@
         <v>86</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>